<commit_message>
added rule source and changes
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
+++ b/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8B64FF-BF9C-4C65-9A5C-7D0416386EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE46B78-5EDF-4653-9F10-1FA02D24020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>The ego vehicle has to stop with respect to a stop sign (sign 206) before it enters the intersection at least for a duration of tslw in front of the associated stop line.</t>
   </si>
   <si>
-    <t>G(at_intersection(ego) &amp; at_traffic_sign(ego,206))-&gt; G[0,t]in_standstill(ego)</t>
-  </si>
-  <si>
     <t>StVO: § 8</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>It is always the case that if the other vehicle is to the left of the ego vehicle and the ego vehicle drives faster than the other vehicle, then the ego vehicle is to the right of a broad lane marking and the other vehicle is to the left of a solid lane marking.</t>
   </si>
   <si>
-    <t>G((left_of(other,ego) &amp; drives_faster(ego,other)) -&gt; (right_of_broad_marking(ego) &amp; left_of_broad_marking(other)))</t>
-  </si>
-  <si>
     <t>the ego vehicle passes a stop line if the stop line is in front of the ego vehicle and is not in front of it at next time step.</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>if ego vehicle is turning left and there is no relevent traffic light for the ego and other vehicle is going to turn right or going straight and other vehicle is onto the oncoming lane of ego then in this case ego shall yield to other vehicle.</t>
   </si>
   <si>
-    <t>G((turning_left(ego) &amp; ~traffic_light(ego) &amp; going_right_or_straight(other) &amp; oncoming_lane(other, ego)) -&gt; yield(ego, other))</t>
-  </si>
-  <si>
     <t>At intersections and junctions ego must yield to the other vehicles coming from right side of ego.</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
   </si>
   <si>
     <t>At intersections and junctions if there is another vehicle in right of ego and there is no traffic light in front of ego then ego must yield to other vehicle, provided there is no traffic sign number 206 in front of ego.</t>
-  </si>
-  <si>
-    <t>G(at_intersection(ego) &amp; right_of(other,ego)&amp;~in_front_of(ego, sign_206)-&gt; (yield(ego,other) ))</t>
   </si>
   <si>
     <t>G(at_intersection(ego) &amp; right_of(other,ego) -&gt; (yield(ego,other)))</t>
@@ -289,9 +277,6 @@
     <t>At intersections with traffic lights, drivers must stop at a red light and may proceed at a green light.</t>
   </si>
   <si>
-    <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F(stop(ego))) ∧ (traffic_light(ego,green) -&gt; F(proceed(ego))))</t>
-  </si>
-  <si>
     <t>At ‘T’ intersections without ‘STOP’ or ‘YIELD’
 signs, yield to traffic and pedestrians on the through
 road. They have the right-of-way</t>
@@ -333,12 +318,6 @@
   </si>
   <si>
     <t>Note we can add restrictions over in how many times maximum they have to procees or stop</t>
-  </si>
-  <si>
-    <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F[0,2](stop(ego))) ∧ (traffic_light(ego,green) -&gt; F[0,2](proceed(ego))))</t>
-  </si>
-  <si>
-    <t>At intersections with traffic lights, drivers must stop at a red light within 3 seconds and may proceed at a green light within 3 seconds.</t>
   </si>
   <si>
     <t>same rule but with more safety property</t>
@@ -376,6 +355,27 @@
   </si>
   <si>
     <t xml:space="preserve">(change_lanes(ego) | turn(ego) | overtake(ego)) -&gt; P[0,t](turn_signals(ego)) </t>
+  </si>
+  <si>
+    <t>G((left_of(other,ego) &amp; drives_faster(ego,other)) -&gt; (in_right_of(ego,broad_lane_marking) &amp; left_of(other,solid_lane_marking)))</t>
+  </si>
+  <si>
+    <t>G((turning_left(ego) &amp; ~traffic_light(ego) &amp; (turn_right(other) | go_straight(other)) &amp; oncoming_lane(other, ego)) -&gt; yield(ego, other))</t>
+  </si>
+  <si>
+    <t>G((at_intersection(ego) &amp; right_of(other,ego)&amp;~in_front_of(sign_206,ego) &amp; ~traffic_light(ego))-&gt; yield(ego,other) )</t>
+  </si>
+  <si>
+    <t>G(at_intersection(ego) &amp; at_traffic_sign(ego,206))-&gt; G[0,tslw]in_standstill(ego)</t>
+  </si>
+  <si>
+    <t>At intersections with traffic lights, drivers must stop at a red light and may proceed at a green light within 3 seconds.</t>
+  </si>
+  <si>
+    <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F(stop(ego))) ∧ (traffic_light(ego,green))) -&gt; F[0,2](proceed(ego))</t>
+  </si>
+  <si>
+    <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F(stop(ego))) ∧ (traffic_light(ego,green))) -&gt; F(proceed(ego))</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <dimension ref="A1:D1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -780,7 +780,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -810,10 +810,10 @@
     </row>
     <row r="9" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -827,270 +827,270 @@
         <v>24</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
change of rule wording and temporal nature.
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
+++ b/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE46B78-5EDF-4653-9F10-1FA02D24020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C02A4A8-6D26-4AF9-93EB-C18CDB69CFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>before overtaking vehicle in front ego shall make sure that other vehicle in behind did not already started to overtake the ego.</t>
-  </si>
-  <si>
-    <t>G(P[0,t](~overtake(vehicle_behind,ego) -&gt; (in_front_of(ego,vehicle_in_front) &amp; overtake(ego,vehicle_in_front))))</t>
   </si>
   <si>
     <t>if there is a traffic light on the ego lane and the traffic color is red, the ego vehicle shall not exceed the stop lane.</t>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F(stop(ego))) ∧ (traffic_light(ego,green))) -&gt; F(proceed(ego))</t>
+  </si>
+  <si>
+    <t>G( (in_front_of(ego,vehicle_in_front) &amp; overtake(ego,vehicle_in_front))-&gt;P[0,t](~overtake(vehicle_behind,ego) ))</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <dimension ref="A1:D1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -739,358 +739,358 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="4" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="C34" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
         <v>78</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rule change for Vcort
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
+++ b/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C02A4A8-6D26-4AF9-93EB-C18CDB69CFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D8234B-CAC6-4CA4-88E6-472261E7A35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>if Ego vehicle in front of other vehicle then it must not brake suddenly without a compelling reason.</t>
-  </si>
-  <si>
-    <t>G(in_front_of(ego,other)-&gt; ~sudden_braking(ego)</t>
   </si>
   <si>
     <t>StVO: § 4 (1)</t>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>G( (in_front_of(ego,vehicle_in_front) &amp; overtake(ego,vehicle_in_front))-&gt;P[0,t](~overtake(vehicle_behind,ego) ))</t>
+  </si>
+  <si>
+    <t>G(in_front_of(ego,other)-&gt; ~sudden_braking(ego))</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -772,7 +772,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -794,57 +794,57 @@
         <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -852,245 +852,245 @@
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="C34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
         <v>77</v>
-      </c>
-      <c r="D34" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update in source file
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
+++ b/TR2MTL_Traffic_Rule_Evaluation_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52783D07-B177-4B35-B0D5-69C1191AE173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD81345-7E8D-4737-B86A-687FB7C58ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,9 +305,6 @@
     <t>same rule but with more safety property</t>
   </si>
   <si>
-    <t>G(~overtake(ego, other_vehicle) -&gt; in_front_of(crosswalk,other_vehicle))</t>
-  </si>
-  <si>
     <t>G(~congestion(ego) |  (~standing(leading) -&gt; ~(stop_main_carriageway(ego) | stop_shoulder_lane(ego) | stop_ramps(ego))))</t>
   </si>
   <si>
@@ -376,6 +373,9 @@
   </si>
   <si>
     <t>G((left_of(other,ego) &amp; drives_faster(ego,other)) -&gt; (in_right_of(ego,broad_lane_marking) &amp; in_left_of(other,solid_lane_marking)))</t>
+  </si>
+  <si>
+    <t>G( in_front_of(crosswalk,other_vehicle)-&gt;~overtake(ego, other_vehicle))</t>
   </si>
 </sst>
 </file>
@@ -708,8 +708,8 @@
   </sheetPr>
   <dimension ref="A1:D1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -734,238 +734,238 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="2" t="s">
+    <row r="22" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
@@ -976,7 +976,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -1064,7 +1064,7 @@
         <v>61</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>72</v>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>72</v>

</xml_diff>